<commit_message>
Neural Network - Início
</commit_message>
<xml_diff>
--- a/Analise_PCA.xlsx
+++ b/Analise_PCA.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan1 (2)" sheetId="2" r:id="rId2"/>
     <sheet name="Gráf1" sheetId="3" r:id="rId3"/>
     <sheet name="Plan2" sheetId="4" r:id="rId4"/>
+    <sheet name="Plan3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="171">
   <si>
     <t>PC1</t>
   </si>
@@ -521,19 +522,47 @@
   </si>
   <si>
     <t>Variação acumulada</t>
+  </si>
+  <si>
+    <t>Autovalores</t>
+  </si>
+  <si>
+    <t>Variação
+acumulada</t>
+  </si>
+  <si>
+    <t>Quantidade
+de componentes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -556,7 +585,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -579,11 +608,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -593,12 +634,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -624,11 +695,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -655,7 +722,7 @@
             <c:idx val="9"/>
             <c:marker>
               <c:symbol val="triangle"/>
-              <c:size val="14"/>
+              <c:size val="10"/>
               <c:spPr>
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
@@ -673,7 +740,7 @@
             <c:idx val="37"/>
             <c:marker>
               <c:symbol val="diamond"/>
-              <c:size val="14"/>
+              <c:size val="10"/>
               <c:spPr>
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
@@ -922,7 +989,7 @@
             <c:numRef>
               <c:f>'Plan1 (2)'!$B$3:$BW$3</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>0.02</c:v>
@@ -1159,11 +1226,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="40407808"/>
-        <c:axId val="40409728"/>
+        <c:axId val="389644288"/>
+        <c:axId val="389646208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40407808"/>
+        <c:axId val="389644288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,7 +1247,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Quantidade de Vetores</a:t>
+                  <a:t>Quantidade de Componentes</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1202,13 +1269,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40409728"/>
+        <c:crossAx val="389646208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40409728"/>
+        <c:axId val="389646208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1235,7 +1302,7 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1249,7 +1316,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40407808"/>
+        <c:crossAx val="389644288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1283,7 +1350,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9638731" cy="6006437"/>
+    <xdr:ext cx="9645570" cy="6016424"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1"/>
@@ -1479,6 +1546,49 @@
         </xdr:spPr>
       </xdr:pic>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>518479</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>388930</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6824029" y="1085850"/>
+          <a:ext cx="8404851" cy="5124450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1773,7 +1883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -3259,15 +3369,14 @@
   <dimension ref="A1:BW8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="B3" sqref="B3:BW3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="72" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="73" max="75" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="72" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="75" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:75" x14ac:dyDescent="0.25">
@@ -3799,226 +3908,226 @@
       <c r="A3" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="16">
         <v>0.02</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="16">
         <v>0.03</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="16">
         <v>0.05</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="16">
         <v>0.06</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="16">
         <v>0.08</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="16">
         <v>0.09</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="16">
         <v>0.11</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="16">
         <v>0.12</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="16">
         <v>0.13</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="16">
         <v>0.15</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="16">
         <v>0.16</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="16">
         <v>0.18</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="16">
         <v>0.19</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="16">
         <v>0.21</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="16">
         <v>0.22</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3" s="16">
         <v>0.24</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="16">
         <v>0.25</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3" s="16">
         <v>0.27</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3" s="16">
         <v>0.28000000000000003</v>
       </c>
-      <c r="U3" s="5">
+      <c r="U3" s="16">
         <v>0.3</v>
       </c>
-      <c r="V3" s="5">
+      <c r="V3" s="16">
         <v>0.31</v>
       </c>
-      <c r="W3" s="5">
+      <c r="W3" s="16">
         <v>0.33</v>
       </c>
-      <c r="X3" s="5">
+      <c r="X3" s="16">
         <v>0.34</v>
       </c>
-      <c r="Y3" s="5">
+      <c r="Y3" s="16">
         <v>0.35</v>
       </c>
-      <c r="Z3" s="5">
+      <c r="Z3" s="16">
         <v>0.37</v>
       </c>
-      <c r="AA3" s="5">
+      <c r="AA3" s="16">
         <v>0.38</v>
       </c>
-      <c r="AB3" s="5">
+      <c r="AB3" s="16">
         <v>0.4</v>
       </c>
-      <c r="AC3" s="5">
+      <c r="AC3" s="16">
         <v>0.41</v>
       </c>
-      <c r="AD3" s="5">
+      <c r="AD3" s="16">
         <v>0.43</v>
       </c>
-      <c r="AE3" s="5">
+      <c r="AE3" s="16">
         <v>0.44</v>
       </c>
-      <c r="AF3" s="5">
+      <c r="AF3" s="16">
         <v>0.45</v>
       </c>
-      <c r="AG3" s="5">
+      <c r="AG3" s="16">
         <v>0.47</v>
       </c>
-      <c r="AH3" s="5">
+      <c r="AH3" s="16">
         <v>0.48</v>
       </c>
-      <c r="AI3" s="5">
+      <c r="AI3" s="16">
         <v>0.5</v>
       </c>
-      <c r="AJ3" s="5">
+      <c r="AJ3" s="16">
         <v>0.51</v>
       </c>
-      <c r="AK3" s="5">
+      <c r="AK3" s="16">
         <v>0.52</v>
       </c>
-      <c r="AL3" s="5">
+      <c r="AL3" s="16">
         <v>0.54</v>
       </c>
-      <c r="AM3" s="5">
+      <c r="AM3" s="16">
         <v>0.55000000000000004</v>
       </c>
-      <c r="AN3" s="5">
+      <c r="AN3" s="16">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AO3" s="5">
+      <c r="AO3" s="16">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AP3" s="5">
+      <c r="AP3" s="16">
         <v>0.59</v>
       </c>
-      <c r="AQ3" s="5">
+      <c r="AQ3" s="16">
         <v>0.61</v>
       </c>
-      <c r="AR3" s="5">
+      <c r="AR3" s="16">
         <v>0.62</v>
       </c>
-      <c r="AS3" s="5">
+      <c r="AS3" s="16">
         <v>0.63</v>
       </c>
-      <c r="AT3" s="5">
+      <c r="AT3" s="16">
         <v>0.65</v>
       </c>
-      <c r="AU3" s="5">
+      <c r="AU3" s="16">
         <v>0.66</v>
       </c>
-      <c r="AV3" s="5">
+      <c r="AV3" s="16">
         <v>0.67</v>
       </c>
-      <c r="AW3" s="5">
+      <c r="AW3" s="16">
         <v>0.69</v>
       </c>
-      <c r="AX3" s="5">
+      <c r="AX3" s="16">
         <v>0.7</v>
       </c>
-      <c r="AY3" s="5">
+      <c r="AY3" s="16">
         <v>0.71</v>
       </c>
-      <c r="AZ3" s="5">
+      <c r="AZ3" s="16">
         <v>0.73</v>
       </c>
-      <c r="BA3" s="5">
+      <c r="BA3" s="16">
         <v>0.74</v>
       </c>
-      <c r="BB3" s="5">
+      <c r="BB3" s="16">
         <v>0.75</v>
       </c>
-      <c r="BC3" s="5">
+      <c r="BC3" s="16">
         <v>0.77</v>
       </c>
-      <c r="BD3" s="5">
+      <c r="BD3" s="16">
         <v>0.78</v>
       </c>
-      <c r="BE3" s="5">
+      <c r="BE3" s="16">
         <v>0.79</v>
       </c>
-      <c r="BF3" s="5">
+      <c r="BF3" s="16">
         <v>0.81</v>
       </c>
-      <c r="BG3" s="5">
+      <c r="BG3" s="16">
         <v>0.82</v>
       </c>
-      <c r="BH3" s="5">
+      <c r="BH3" s="16">
         <v>0.83</v>
       </c>
-      <c r="BI3" s="5">
+      <c r="BI3" s="16">
         <v>0.85</v>
       </c>
-      <c r="BJ3" s="5">
+      <c r="BJ3" s="16">
         <v>0.86</v>
       </c>
-      <c r="BK3" s="5">
+      <c r="BK3" s="16">
         <v>0.87</v>
       </c>
-      <c r="BL3" s="5">
+      <c r="BL3" s="16">
         <v>0.88</v>
       </c>
-      <c r="BM3" s="5">
+      <c r="BM3" s="16">
         <v>0.9</v>
       </c>
-      <c r="BN3" s="5">
+      <c r="BN3" s="16">
         <v>0.91</v>
       </c>
-      <c r="BO3" s="5">
+      <c r="BO3" s="16">
         <v>0.92</v>
       </c>
-      <c r="BP3" s="5">
+      <c r="BP3" s="16">
         <v>0.94</v>
       </c>
-      <c r="BQ3" s="5">
+      <c r="BQ3" s="16">
         <v>0.95</v>
       </c>
-      <c r="BR3" s="5">
+      <c r="BR3" s="16">
         <v>0.96</v>
       </c>
-      <c r="BS3" s="5">
+      <c r="BS3" s="16">
         <v>0.97</v>
       </c>
-      <c r="BT3" s="5">
+      <c r="BT3" s="16">
         <v>0.99</v>
       </c>
-      <c r="BU3" s="5">
+      <c r="BU3" s="16">
         <v>1</v>
       </c>
-      <c r="BV3" s="5">
+      <c r="BV3" s="16">
         <v>1</v>
       </c>
-      <c r="BW3" s="5">
+      <c r="BW3" s="16">
         <v>1</v>
       </c>
     </row>
@@ -4026,226 +4135,226 @@
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>1.1299999999999999</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>1.1100000000000001</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <v>1.1100000000000001</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="5">
         <v>1.1100000000000001</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="5">
         <v>1.1100000000000001</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="5">
         <v>1.1100000000000001</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="5">
         <v>1.0900000000000001</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="5">
         <v>1.0900000000000001</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="5">
         <v>1.0900000000000001</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="5">
         <v>1.08</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="5">
         <v>1.08</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="5">
         <v>1.08</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="5">
         <v>1.08</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4" s="5">
         <v>1.07</v>
       </c>
-      <c r="W4" s="2">
+      <c r="W4" s="5">
         <v>1.07</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4" s="5">
         <v>1.07</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Y4" s="5">
         <v>1.07</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="Z4" s="5">
         <v>1.06</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AA4" s="5">
         <v>1.06</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AB4" s="5">
         <v>1.06</v>
       </c>
-      <c r="AC4" s="2">
+      <c r="AC4" s="5">
         <v>1.06</v>
       </c>
-      <c r="AD4" s="2">
+      <c r="AD4" s="5">
         <v>1.05</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AE4" s="5">
         <v>1.05</v>
       </c>
-      <c r="AF4" s="2">
+      <c r="AF4" s="5">
         <v>1.04</v>
       </c>
-      <c r="AG4" s="2">
+      <c r="AG4" s="5">
         <v>1.04</v>
       </c>
-      <c r="AH4" s="2">
+      <c r="AH4" s="5">
         <v>1.03</v>
       </c>
-      <c r="AI4" s="2">
+      <c r="AI4" s="5">
         <v>1.03</v>
       </c>
-      <c r="AJ4" s="2">
+      <c r="AJ4" s="5">
         <v>1.02</v>
       </c>
-      <c r="AK4" s="2">
+      <c r="AK4" s="5">
         <v>1.02</v>
       </c>
-      <c r="AL4" s="2">
+      <c r="AL4" s="5">
         <v>1.01</v>
       </c>
-      <c r="AM4" s="2">
+      <c r="AM4" s="5">
         <v>1</v>
       </c>
-      <c r="AN4" s="2">
+      <c r="AN4" s="5">
         <v>1</v>
       </c>
-      <c r="AO4" s="2">
+      <c r="AO4" s="5">
         <v>1</v>
       </c>
-      <c r="AP4" s="2">
+      <c r="AP4" s="5">
         <v>1</v>
       </c>
-      <c r="AQ4" s="2">
+      <c r="AQ4" s="5">
         <v>1</v>
       </c>
-      <c r="AR4" s="2">
+      <c r="AR4" s="5">
         <v>1</v>
       </c>
-      <c r="AS4" s="2">
+      <c r="AS4" s="5">
         <v>1</v>
       </c>
-      <c r="AT4" s="2">
+      <c r="AT4" s="5">
         <v>1</v>
       </c>
-      <c r="AU4" s="2">
+      <c r="AU4" s="5">
         <v>1</v>
       </c>
-      <c r="AV4" s="2">
+      <c r="AV4" s="5">
         <v>0.99</v>
       </c>
-      <c r="AW4" s="2">
+      <c r="AW4" s="5">
         <v>0.99</v>
       </c>
-      <c r="AX4" s="2">
+      <c r="AX4" s="5">
         <v>0.99</v>
       </c>
-      <c r="AY4" s="2">
+      <c r="AY4" s="5">
         <v>0.99</v>
       </c>
-      <c r="AZ4" s="2">
+      <c r="AZ4" s="5">
         <v>0.99</v>
       </c>
-      <c r="BA4" s="2">
+      <c r="BA4" s="5">
         <v>0.99</v>
       </c>
-      <c r="BB4" s="2">
+      <c r="BB4" s="5">
         <v>0.99</v>
       </c>
-      <c r="BC4" s="2">
+      <c r="BC4" s="5">
         <v>0.98</v>
       </c>
-      <c r="BD4" s="2">
+      <c r="BD4" s="5">
         <v>0.98</v>
       </c>
-      <c r="BE4" s="2">
+      <c r="BE4" s="5">
         <v>0.98</v>
       </c>
-      <c r="BF4" s="2">
+      <c r="BF4" s="5">
         <v>0.98</v>
       </c>
-      <c r="BG4" s="2">
+      <c r="BG4" s="5">
         <v>0.97</v>
       </c>
-      <c r="BH4" s="2">
+      <c r="BH4" s="5">
         <v>0.97</v>
       </c>
-      <c r="BI4" s="2">
+      <c r="BI4" s="5">
         <v>0.97</v>
       </c>
-      <c r="BJ4" s="2">
+      <c r="BJ4" s="5">
         <v>0.97</v>
       </c>
-      <c r="BK4" s="2">
+      <c r="BK4" s="5">
         <v>0.97</v>
       </c>
-      <c r="BL4" s="2">
+      <c r="BL4" s="5">
         <v>0.96</v>
       </c>
-      <c r="BM4" s="2">
+      <c r="BM4" s="5">
         <v>0.96</v>
       </c>
-      <c r="BN4" s="2">
+      <c r="BN4" s="5">
         <v>0.96</v>
       </c>
-      <c r="BO4" s="2">
+      <c r="BO4" s="5">
         <v>0.96</v>
       </c>
-      <c r="BP4" s="2">
+      <c r="BP4" s="5">
         <v>0.96</v>
       </c>
-      <c r="BQ4" s="2">
+      <c r="BQ4" s="5">
         <v>0.95</v>
       </c>
-      <c r="BR4" s="2">
+      <c r="BR4" s="5">
         <v>0.95</v>
       </c>
-      <c r="BS4" s="2">
+      <c r="BS4" s="5">
         <v>0.94</v>
       </c>
-      <c r="BT4" s="2">
+      <c r="BT4" s="5">
         <v>0.92</v>
       </c>
-      <c r="BU4" s="2">
+      <c r="BU4" s="5">
         <v>0.9</v>
       </c>
-      <c r="BV4" s="2">
+      <c r="BV4" s="5">
         <v>0.03</v>
       </c>
-      <c r="BW4" s="2">
+      <c r="BW4" s="5">
         <v>0.03</v>
       </c>
     </row>
@@ -5167,7 +5276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -5176,4 +5285,71 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.10229</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>38</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1.0016400000000001</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
+        <v>39</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.99978</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>